<commit_message>
Agregar videos, completo! Falta eliminar y editar
</commit_message>
<xml_diff>
--- a/flaskr/static/files/Usuarios.xlsx
+++ b/flaskr/static/files/Usuarios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,6 +649,48 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Pepe</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Lopez</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PepeL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>12121212</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pepel@ejemplo.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fkjdfhaskjfhashfhasfadfhjasdfhads</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>44300</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Sin Adquirir</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifique la variable de entorno para la sudida de videos
</commit_message>
<xml_diff>
--- a/flaskr/static/files/Usuarios.xlsx
+++ b/flaskr/static/files/Usuarios.xlsx
@@ -672,7 +672,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>pepel@ejemplo.com</t>
+          <t>pepe@ejemplo.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sin Adquirir</t>
+          <t>Adquirido</t>
         </is>
       </c>
     </row>

</xml_diff>